<commit_message>
Host viewer and elimate floating point computation, printf. the bin size has been reduced to 6K
</commit_message>
<xml_diff>
--- a/scratch.xlsx
+++ b/scratch.xlsx
@@ -912,375 +912,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Rt</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$111</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="110"/>
-                <c:pt idx="0">
-                  <c:v>33620.603721435742</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>31893.138272305434</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30266.034194017953</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28732.835517560583</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>27287.539531911738</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25924.56241959352</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24638.70768276219</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>23425.137118719744</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22279.344125776763</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21197.129140324207</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20174.57702398485</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>19208.036236013788</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>18294.099640871082</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>17429.586814247774</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16611.527722935953</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15837.147664908136</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>15103.853365929419</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>14409.220138062792</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>13750.980013633698</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>13127.010775676536</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>12535.32581266281</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11974.064731474306</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11441.484668193882</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>10935.952241391826</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>10455.936097237052</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9566.7964253785212</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9155.0606176022357</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>8763.6050744872282</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>8391.3144275502273</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8037.1406869731372</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>7700.09882366077</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7379.2626628761145</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7073.7610659870961</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>6782.7743787355321</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>6505.5311261565666</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>6241.304935849771</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>5989.4116727455057</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>5749.2067698310466</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>5520.0827405136479</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>5301.4668594096684</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>5092.8189993696833</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4893.62961348718</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4703.4178516995044</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>4521.7298023814565</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4348.1368500594717</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4182.2341410439949</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>4023.6391493935303</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>3871.9903361908941</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>3726.945895634597</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>3588.182581929083</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>3455.3946114014111</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>3328.2926346803315</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>3206.602774151228</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>3090.0657222480427</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2978.4358964646267</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>2871.48064726449</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>2768.9795153419145</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>2670.7235349405078</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>2576.5145801693689</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>2486.1647514733818</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2399.4957996144262</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>2316.3385847055865</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>2236.5325680118708</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>2159.925334389869</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>2086.3721433859669</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>2015.7355071489537</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>1947.8847934394441</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1882.6958521356758</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>1820.0506637440094</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1759.8370085233807</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1701.9481549266641</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>1646.2825661488762</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1592.7436236529284</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1541.2393666187754</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1491.682246331595</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>1443.9888945894415</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1398.0799052713089</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1353.8796282625538</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1311.3159749870022</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>1270.3202348436205</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1230.8269018910289</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>1192.7735111652521</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>1156.1004840554915</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1120.7509821993378</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>1086.6707693930255</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>1053.8080810441725</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>1022.1135007242613</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>991.53984340578097</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>962.04204499490004</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>933.57705779475566</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>906.10375155695078</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>879.58281980005268</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>853.97669109353592</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>829.24944502410733</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>805.36673257853829</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>782.29570069330578</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>760.00492073640328</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>738.4643207007814</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>717.64512090214896</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>697.51977298618806</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>678.06190206183987</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>659.24625178819122</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>641.04863225265444</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>623.44587048764549</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>606.41576348196213</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>589.93703355138325</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>573.98928594092331</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>558.55296853852633</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>543.60933358693057</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$D$1</c:f>
@@ -2727,7 +2360,7 @@
   <dimension ref="A1:R111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J12"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>